<commit_message>
Minor fixes - FDA-96, FDA-98, FDA-106
</commit_message>
<xml_diff>
--- a/static/fields/deviceevent_reference.xlsx
+++ b/static/fields/deviceevent_reference.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C46D42-BAD6-244F-9FCF-9029120D2D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="60" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="3440" yWindow="460" windowWidth="25360" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_event_fields" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="251">
   <si>
     <t>Field Name</t>
   </si>
@@ -1123,11 +1129,17 @@
   <si>
     <t>The classification regulation in the Code of Federal Regulations (CFR) under which the device is identified, described, and formally classified (Code of Federal regulations Title 21, 862.00 through 892.00). The classification regulation covers various aspects of design, clinical evaluation, manufacturing, packaging, labeling, and postmarket surveillance of the specific medical device.</t>
   </si>
+  <si>
+    <t>product_problems</t>
+  </si>
+  <si>
+    <t>The product problems that were reported to the FDA if there was a concern about the quality, authenticity, performance, or safety of any medication or device.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1404,7 +1416,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1430,6 +1442,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="211">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1646,6 +1659,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1970,26 +1991,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B112" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="134.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="105">
+    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -2017,1631 +2038,1646 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="120">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>249</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="180">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="135">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="225">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="90">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="255" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="105">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="105">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="135">
-      <c r="A16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="105">
+    <row r="17" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="409">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="135">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="120">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="C21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60">
-      <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5" t="s">
+      <c r="C24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="60">
-      <c r="A24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="60">
+    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="75">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="45">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="60">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="150">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="150">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="C36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="409">
-      <c r="A36" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="45">
+    <row r="37" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="195">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="C39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45">
-      <c r="A39" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="45">
+    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>55</v>
+      <c r="B42" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="45">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B47" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="C48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="45">
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="255">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="289" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="C52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30">
-      <c r="A52" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="45">
+    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="60">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="210">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="C57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="135">
-      <c r="A57" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30">
+    <row r="58" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="120">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="135">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="409">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D64" s="5" t="s">
+      <c r="C65" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="45">
-      <c r="A65" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="45">
+    <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="45">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="45">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="45">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="C72" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="45">
-      <c r="A72" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="45">
+    <row r="73" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="45">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="75">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="45">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="45">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="75">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="45">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="45">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="45">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="45">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="45">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="75">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="45">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="45">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="45">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="45">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="45">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="45">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="45">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="60">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="75">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="45">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="45">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="45">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="45">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B107" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D107" s="5" t="s">
+      <c r="C108" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="45">
-      <c r="A108" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="240">
+    <row r="109" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B109" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D109" s="5" t="s">
+      <c r="C110" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="45">
-      <c r="A110" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="45">
+    <row r="111" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="120">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B112" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B113" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D112" s="5" t="s">
+      <c r="C113" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D113" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="135">
-      <c r="A113" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="45">
+    <row r="114" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="60">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="45">
+        <v>3</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D118" s="5" t="s">
+    </row>
+    <row r="119" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D119" s="5" t="s">
         <v>248</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="21" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Adding `patient.patient_problems` to Device Events (MAUDE).
</commit_message>
<xml_diff>
--- a/static/fields/deviceevent_reference.xlsx
+++ b/static/fields/deviceevent_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D5B2F4-0B6D-934E-A828-396F8530FF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB8EED5-B43A-7242-AEFD-DBFCFDEA5F9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="460" windowWidth="25360" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="460" windowWidth="34060" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_event_fields" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="253">
   <si>
     <t>Field Name</t>
   </si>
@@ -1134,6 +1134,13 @@
   </si>
   <si>
     <t>The product problems that were reported to the FDA if there was a concern about the quality, authenticity, performance, or safety of any medication or device.</t>
+  </si>
+  <si>
+    <t>patient.patient_problems</t>
+  </si>
+  <si>
+    <t>Describes actual adverse effects on the patient that may be related to the device problem observed during the reported event.
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
 </sst>
 </file>
@@ -1995,10 +2002,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2710,228 +2717,228 @@
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="289" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>64</v>
+        <v>251</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="289" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="C58" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="C66" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2939,13 +2946,13 @@
         <v>80</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2953,13 +2960,13 @@
         <v>80</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2967,13 +2974,13 @@
         <v>80</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2981,13 +2988,13 @@
         <v>80</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2995,13 +3002,13 @@
         <v>80</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3009,27 +3016,27 @@
         <v>80</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3037,13 +3044,13 @@
         <v>88</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3051,13 +3058,13 @@
         <v>88</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3065,13 +3072,13 @@
         <v>88</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3079,13 +3086,13 @@
         <v>88</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3093,13 +3100,13 @@
         <v>88</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3107,13 +3114,13 @@
         <v>88</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3121,41 +3128,41 @@
         <v>88</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3163,13 +3170,13 @@
         <v>88</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3177,13 +3184,13 @@
         <v>88</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3191,41 +3198,41 @@
         <v>88</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3233,13 +3240,13 @@
         <v>88</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3247,13 +3254,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3261,13 +3268,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3275,13 +3282,13 @@
         <v>88</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3289,41 +3296,41 @@
         <v>88</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3331,13 +3338,13 @@
         <v>88</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3345,13 +3352,13 @@
         <v>88</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3359,13 +3366,13 @@
         <v>88</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3373,13 +3380,13 @@
         <v>88</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3387,13 +3394,13 @@
         <v>88</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3401,27 +3408,27 @@
         <v>88</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>232</v>
+        <v>173</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3429,27 +3436,27 @@
         <v>88</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3457,27 +3464,27 @@
         <v>88</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3485,27 +3492,27 @@
         <v>88</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3513,55 +3520,55 @@
         <v>88</v>
       </c>
       <c r="B108" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D108" s="5" t="s">
+      <c r="C109" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B110" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B111" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D110" s="5" t="s">
+      <c r="C111" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3569,107 +3576,121 @@
         <v>127</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B113" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B114" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D113" s="5" t="s">
+      <c r="C114" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D114" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D119" s="5" t="s">
+    </row>
+    <row r="120" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120" s="5" t="s">
         <v>248</v>
       </c>
     </row>
@@ -3677,7 +3698,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="29" fitToWidth="4" fitToHeight="4" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Updated device event names to support changes in final release.
</commit_message>
<xml_diff>
--- a/static/fields/deviceevent_reference.xlsx
+++ b/static/fields/deviceevent_reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25811"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{3BB8EED5-B43A-7242-AEFD-DBFCFDEA5F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCC66179-2E29-4ED4-A70E-32624FDEE962}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{3BB8EED5-B43A-7242-AEFD-DBFCFDEA5F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4685D66-C430-43E0-A9EF-BB6E7AF03541}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="460" windowWidth="34060" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,13 +331,13 @@
 This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
   </si>
   <si>
-    <t>device.gudid_deviceid</t>
+    <t>device.udi_di</t>
   </si>
   <si>
     <t>A unique numeric or alphanumeric code specific to a device version or model.</t>
   </si>
   <si>
-    <t>device.redacted_udi</t>
+    <t>device.udi_public</t>
   </si>
   <si>
     <t>Includes both the UDI-DI and the parts of the Production identifier (PI) that would not identify an individual patient. The Production Identifier is  a conditional, variable portion of a UDI that identifies one or more of the following when included on the label of a device and may include: 1) lot or batch number within which a device was manufactured, 2) serial number of a specific device, 3) expiration date of a specific device, 4) date a specific device was manufactured, and 5) distinct identification code required by §1271.290(c) for a human cell, tissue, or cellular and tissue-based product (HCT/P) regulated as a device.</t>
@@ -1474,135 +1474,172 @@
     </xf>
   </cellXfs>
   <cellStyles count="211">
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
@@ -1610,7 +1647,6 @@
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
@@ -1618,7 +1654,6 @@
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
@@ -1626,64 +1661,29 @@
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2027,7 +2027,7 @@
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>

</xml_diff>

<commit_message>
Added patient demographic fields (age, sex, weight, ethnicity, and race) to the Device Event endpoint since these fields have now become available in the MAUDE dataset at FDA.
</commit_message>
<xml_diff>
--- a/static/fields/deviceevent_reference.xlsx
+++ b/static/fields/deviceevent_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{3BB8EED5-B43A-7242-AEFD-DBFCFDEA5F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4685D66-C430-43E0-A9EF-BB6E7AF03541}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C997D7E-D2EF-4B49-A2C8-9E2460E20DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="460" windowWidth="34060" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="38120" windowHeight="19980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_event_fields" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="267">
   <si>
     <t>Section</t>
   </si>
@@ -1165,12 +1165,42 @@
   <si>
     <t>The classification regulation in the Code of Federal Regulations (CFR) under which the device is identified, described, and formally classified (Code of Federal regulations Title 21, 862.00 through 892.00). The classification regulation covers various aspects of design, clinical evaluation, manufacturing, packaging, labeling, and postmarket surveillance of the specific medical device.</t>
   </si>
+  <si>
+    <t>patient.patient_age</t>
+  </si>
+  <si>
+    <t>patient.patient_sex</t>
+  </si>
+  <si>
+    <t>patient.patient_weight</t>
+  </si>
+  <si>
+    <t>patient.patient_ethnicity</t>
+  </si>
+  <si>
+    <t>patient.patient_race</t>
+  </si>
+  <si>
+    <t>Patient's age. This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
+  <si>
+    <t>Patient's gender. This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
+  <si>
+    <t>Patient's weight. This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
+  <si>
+    <t>Patient's ethnicity. This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
+  <si>
+    <t>Patient's race. This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1446,7 +1476,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1472,6 +1502,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="211">
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
@@ -2024,22 +2055,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="134.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="3"/>
+    <col min="4" max="4" width="134.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2053,7 +2084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="119.1">
+    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +2098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="135.94999999999999">
+    <row r="4" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2095,7 +2126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.100000000000001">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2109,7 +2140,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="33.950000000000003">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2123,7 +2154,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.100000000000001">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2168,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.100000000000001">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2151,7 +2182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="204">
+    <row r="9" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -2165,7 +2196,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="51">
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -2179,7 +2210,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51">
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -2193,7 +2224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="153">
+    <row r="12" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -2207,7 +2238,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="255">
+    <row r="13" spans="1:4" ht="255" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -2221,7 +2252,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="102">
+    <row r="14" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -2235,7 +2266,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="119.1">
+    <row r="15" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -2249,7 +2280,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="119.1">
+    <row r="16" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -2263,7 +2294,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="153">
+    <row r="17" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
@@ -2277,7 +2308,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="119.1">
+    <row r="18" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
@@ -2291,7 +2322,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="409.6">
+    <row r="19" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
@@ -2305,7 +2336,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="153">
+    <row r="20" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -2319,7 +2350,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="135.94999999999999">
+    <row r="21" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>37</v>
       </c>
@@ -2333,7 +2364,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="68.099999999999994">
+    <row r="22" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>48</v>
       </c>
@@ -2347,7 +2378,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.100000000000001">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
@@ -2361,7 +2392,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.100000000000001">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
@@ -2375,7 +2406,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="68.099999999999994">
+    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>55</v>
       </c>
@@ -2389,7 +2420,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="51">
+    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>55</v>
       </c>
@@ -2403,7 +2434,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5">
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>55</v>
       </c>
@@ -2417,7 +2448,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="64.5">
+    <row r="28" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
@@ -2431,7 +2462,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="84.95">
+    <row r="29" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>55</v>
       </c>
@@ -2445,7 +2476,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="51">
+    <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>55</v>
       </c>
@@ -2459,7 +2490,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="51">
+    <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>55</v>
       </c>
@@ -2473,7 +2504,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="51">
+    <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>55</v>
       </c>
@@ -2487,7 +2518,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="68.099999999999994">
+    <row r="33" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
@@ -2501,7 +2532,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.100000000000001">
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>55</v>
       </c>
@@ -2515,7 +2546,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="33.950000000000003">
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>55</v>
       </c>
@@ -2529,7 +2560,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="170.1">
+    <row r="36" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>55</v>
       </c>
@@ -2543,7 +2574,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.100000000000001">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>55</v>
       </c>
@@ -2557,7 +2588,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="153">
+    <row r="38" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
@@ -2571,7 +2602,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="409.6">
+    <row r="39" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>84</v>
       </c>
@@ -2585,7 +2616,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="51">
+    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>84</v>
       </c>
@@ -2599,7 +2630,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="221.1">
+    <row r="41" spans="1:4" ht="221" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>84</v>
       </c>
@@ -2613,7 +2644,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="51">
+    <row r="42" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>91</v>
       </c>
@@ -2627,7 +2658,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="51">
+    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
@@ -2641,7 +2672,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="51">
+    <row r="44" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>91</v>
       </c>
@@ -2655,7 +2686,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="51">
+    <row r="45" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>91</v>
       </c>
@@ -2669,7 +2700,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="51">
+    <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>91</v>
       </c>
@@ -2683,7 +2714,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="51">
+    <row r="47" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>91</v>
       </c>
@@ -2697,7 +2728,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="51">
+    <row r="48" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>91</v>
       </c>
@@ -2711,7 +2742,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="51">
+    <row r="49" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>91</v>
       </c>
@@ -2725,7 +2756,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="51">
+    <row r="50" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>91</v>
       </c>
@@ -2739,7 +2770,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.100000000000001">
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>110</v>
       </c>
@@ -2753,7 +2784,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="51">
+    <row r="52" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>110</v>
       </c>
@@ -2767,984 +2798,1053 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="51">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>115</v>
+      <c r="B53" s="9" t="s">
+        <v>257</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="288.95">
+        <v>6</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>117</v>
+      <c r="B54" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="51">
+        <v>6</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="289" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D60" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.100000000000001">
-      <c r="A56" s="3" t="s">
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="C61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="51">
-      <c r="A57" s="3" t="s">
+    <row r="62" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="C62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="68.099999999999994">
-      <c r="A58" s="3" t="s">
+    <row r="63" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="5" t="s">
+      <c r="C63" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="51">
-      <c r="A59" s="3" t="s">
+    <row r="64" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="5" t="s">
+      <c r="C64" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="221.1">
-      <c r="A60" s="3" t="s">
+    <row r="65" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="5" t="s">
+      <c r="C65" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="153">
-      <c r="A61" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="33.950000000000003">
-      <c r="A62" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="17.100000000000001">
-      <c r="A63" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="135.94999999999999">
-      <c r="A64" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="17.100000000000001">
-      <c r="A65" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="153">
+    <row r="66" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="17.100000000000001">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="409.6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="5" t="s">
+      <c r="C73" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="51">
-      <c r="A69" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="51">
-      <c r="A70" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="51">
-      <c r="A71" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="51">
-      <c r="A72" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="51">
-      <c r="A73" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="51">
+    <row r="74" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="51">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="5" t="s">
+      <c r="C80" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="51">
-      <c r="A76" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="51">
-      <c r="A77" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="51">
-      <c r="A78" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="51">
-      <c r="A79" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="51">
-      <c r="A80" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="51">
+    <row r="81" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="51">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="51">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="68.099999999999994">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="51">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="51">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="51">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="51">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="68.099999999999994">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="51">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="51">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="51">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="51">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="51">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="51">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="68.099999999999994">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="51">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="51">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="51">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="51">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="51">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="51">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="51">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="68.099999999999994">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="68.099999999999994">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="51">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="51">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="17.100000000000001">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="17.100000000000001">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="51">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="51">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B111" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" s="5" t="s">
+      <c r="C116" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" s="5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="33.950000000000003">
-      <c r="A112" s="3" t="s">
+    <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D112" s="5" t="s">
+      <c r="C117" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="272.10000000000002">
-      <c r="A113" s="3" t="s">
+    <row r="118" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D113" s="5" t="s">
+      <c r="C118" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="51">
-      <c r="A114" s="3" t="s">
+    <row r="119" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D114" s="5" t="s">
+      <c r="C119" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="51">
-      <c r="A115" s="3" t="s">
+    <row r="120" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D115" s="5" t="s">
+      <c r="C120" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="135.94999999999999">
-      <c r="A116" s="3" t="s">
+    <row r="121" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D116" s="5" t="s">
+      <c r="C121" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="153">
-      <c r="A117" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="51">
-      <c r="A118" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="17.100000000000001">
-      <c r="A119" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="68.099999999999994">
-      <c r="A120" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D120" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="51">
+    <row r="122" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>245</v>
       </c>
       <c r="B122" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B127" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C127" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="D127" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.75"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions gridLines="1"/>

</xml_diff>